<commit_message>
Ag Census: add owner-operated vars, and fix age and newcomer units
</commit_message>
<xml_diff>
--- a/data/nass/variables.xlsx
+++ b/data/nass/variables.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ca2cc\county_dataset\data\nass\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matthewkling/Documents/barracuda/CA2CC/ca2cc-county/data/nass/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A3632D7-9800-4B7F-B1DB-07005503B664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A53307A-92EC-6444-8D2A-22AEB2C4856D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{9904CD43-FAE1-4C75-AFDC-07B1C411E0EA}"/>
+    <workbookView xWindow="3600" yWindow="3240" windowWidth="45600" windowHeight="23840" xr2:uid="{9904CD43-FAE1-4C75-AFDC-07B1C411E0EA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="572" uniqueCount="203">
   <si>
     <t>FARM OPERATIONS - NUMBER OF OPERATIONS</t>
   </si>
@@ -613,6 +613,27 @@
   </si>
   <si>
     <t>organic_transitioning</t>
+  </si>
+  <si>
+    <t>producers</t>
+  </si>
+  <si>
+    <t>FARM OPERATIONS, ORGANIZATION, GT 50 PCT OWNERSHIP HELD BY PRINCIPAL OPERATOR &amp; RELATED PERSONS - NUMBER OF OPERATIONS</t>
+  </si>
+  <si>
+    <t>FARM OPERATIONS, ORGANIZATION, GT 50 PCT OWNERSHIP HELD BY ONE PRODUCERS HOUSEHOLD &amp; EXTENDED FAMILY - OPERATIONS WITH AREA OPERATED</t>
+  </si>
+  <si>
+    <t>FARM OPERATIONS, ORGANIZATION, GT 50 PCT OWNERSHIP HELD BY PRINCIPAL OPERATOR &amp; RELATED PERSONS - ACRES OPERATED</t>
+  </si>
+  <si>
+    <t>FARM OPERATIONS, ORGANIZATION, GT 50 PCT OWNERSHIP HELD BY ONE PRODUCERS HOUSEHOLD &amp; EXTENDED FAMILY - ACRES OPERATED</t>
+  </si>
+  <si>
+    <t>owner_operated_ops</t>
+  </si>
+  <si>
+    <t>owner_operated_acres</t>
   </si>
 </sst>
 </file>
@@ -964,25 +985,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51E3E093-98A5-40BD-BF81-61CE43BBDA88}">
-  <dimension ref="A1:K87"/>
+  <dimension ref="A1:K91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="3" max="3" width="70" customWidth="1"/>
-    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="9.1640625" customWidth="1"/>
     <col min="5" max="5" width="9" customWidth="1"/>
-    <col min="6" max="6" width="38.85546875" customWidth="1"/>
-    <col min="7" max="7" width="24.28515625" customWidth="1"/>
-    <col min="8" max="8" width="21.42578125" customWidth="1"/>
-    <col min="9" max="9" width="12.7109375" customWidth="1"/>
-    <col min="11" max="11" width="25.42578125" customWidth="1"/>
+    <col min="6" max="6" width="38.83203125" customWidth="1"/>
+    <col min="7" max="7" width="24.33203125" customWidth="1"/>
+    <col min="8" max="8" width="21.5" customWidth="1"/>
+    <col min="9" max="9" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="25.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>6</v>
       </c>
@@ -1017,7 +1038,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>2</v>
       </c>
@@ -1043,7 +1064,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1072,7 +1093,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1101,7 +1122,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1127,7 +1148,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1156,7 +1177,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1182,7 +1203,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1211,7 +1232,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1237,7 +1258,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1266,7 +1287,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1295,7 +1316,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1321,7 +1342,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1350,7 +1371,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1376,7 +1397,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1402,7 +1423,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -1428,7 +1449,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -1457,7 +1478,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -1486,7 +1507,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -1509,7 +1530,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1538,7 +1559,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>2</v>
       </c>
@@ -1561,7 +1582,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>2</v>
       </c>
@@ -1590,7 +1611,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>2</v>
       </c>
@@ -1613,7 +1634,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>2</v>
       </c>
@@ -1642,7 +1663,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -1665,7 +1686,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -1694,27 +1715,24 @@
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
       <c r="B27">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
+        <v>197</v>
       </c>
       <c r="E27">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="G27" t="s">
-        <v>154</v>
-      </c>
-      <c r="H27" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="I27" t="s">
         <v>136</v>
@@ -1723,27 +1741,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
       <c r="B28">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C28" t="s">
-        <v>19</v>
+        <v>198</v>
       </c>
       <c r="E28">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F28" t="s">
-        <v>127</v>
+        <v>201</v>
       </c>
       <c r="G28" t="s">
-        <v>154</v>
-      </c>
-      <c r="H28" t="s">
-        <v>84</v>
+        <v>201</v>
       </c>
       <c r="I28" t="s">
         <v>136</v>
@@ -1752,85 +1767,85 @@
         <v>138</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
       <c r="B29">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C29" t="s">
-        <v>21</v>
+        <v>199</v>
       </c>
       <c r="E29">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F29" t="s">
-        <v>128</v>
+        <v>202</v>
       </c>
       <c r="G29" t="s">
-        <v>155</v>
-      </c>
-      <c r="H29" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="I29" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J29" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K29" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
       <c r="B30">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C30" t="s">
-        <v>22</v>
+        <v>200</v>
       </c>
       <c r="E30">
         <v>2017</v>
       </c>
       <c r="F30" t="s">
-        <v>129</v>
+        <v>202</v>
       </c>
       <c r="G30" t="s">
-        <v>156</v>
-      </c>
-      <c r="H30" t="s">
-        <v>161</v>
+        <v>202</v>
       </c>
       <c r="I30" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J30" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K30" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
       <c r="B31">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C31" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E31">
         <v>2017</v>
       </c>
       <c r="F31" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="H31" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
@@ -1839,27 +1854,27 @@
         <v>138</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
       <c r="B32">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E32">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="G32" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="H32" t="s">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s">
         <v>136</v>
@@ -1868,24 +1883,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
       <c r="B33">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E33">
         <v>2017</v>
       </c>
       <c r="F33" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G33" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H33" t="s">
         <v>161</v>
@@ -1897,24 +1912,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2</v>
       </c>
       <c r="B34">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="C34" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="E34">
         <v>2017</v>
       </c>
       <c r="F34" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G34" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H34" t="s">
         <v>161</v>
@@ -1926,24 +1941,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
       <c r="B35">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C35" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="E35">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F35" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="G35" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="H35" t="s">
         <v>161</v>
@@ -1955,24 +1970,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
       <c r="B36">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C36" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E36">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F36" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="G36" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="H36" t="s">
         <v>161</v>
@@ -1984,24 +1999,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
       <c r="B37">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C37" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="E37">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F37" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="G37" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H37" t="s">
         <v>161</v>
@@ -2013,24 +2028,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
       <c r="B38">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C38" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E38">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F38" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="G38" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="H38" t="s">
         <v>161</v>
@@ -2042,24 +2057,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
       <c r="B39">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C39" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E39">
         <v>2012</v>
       </c>
       <c r="F39" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G39" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H39" t="s">
         <v>161</v>
@@ -2071,24 +2086,24 @@
         <v>138</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
       <c r="B40">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C40" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="E40">
         <v>2012</v>
       </c>
       <c r="F40" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G40" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="H40" t="s">
         <v>161</v>
@@ -2100,27 +2115,27 @@
         <v>138</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
       <c r="B41">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="C41" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
       <c r="E41">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F41" t="s">
-        <v>94</v>
+        <v>130</v>
       </c>
       <c r="G41" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
       <c r="H41" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I41" t="s">
         <v>136</v>
@@ -2129,27 +2144,27 @@
         <v>138</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
       <c r="B42">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="C42" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="E42">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F42" t="s">
-        <v>95</v>
+        <v>131</v>
       </c>
       <c r="G42" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="H42" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I42" t="s">
         <v>136</v>
@@ -2158,27 +2173,27 @@
         <v>138</v>
       </c>
     </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>2</v>
       </c>
       <c r="B43">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C43" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="E43">
         <v>2012</v>
       </c>
       <c r="F43" t="s">
-        <v>94</v>
+        <v>132</v>
       </c>
       <c r="G43" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H43" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I43" t="s">
         <v>136</v>
@@ -2187,27 +2202,27 @@
         <v>138</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>2</v>
       </c>
       <c r="B44">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="C44" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="E44">
         <v>2012</v>
       </c>
       <c r="F44" t="s">
-        <v>95</v>
+        <v>133</v>
       </c>
       <c r="G44" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="H44" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="I44" t="s">
         <v>136</v>
@@ -2216,7 +2231,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>2</v>
       </c>
@@ -2224,28 +2239,28 @@
         <v>45</v>
       </c>
       <c r="C45" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="E45">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F45" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G45" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H45" t="s">
         <v>162</v>
       </c>
       <c r="I45" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J45" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>2</v>
       </c>
@@ -2253,28 +2268,28 @@
         <v>45</v>
       </c>
       <c r="C46" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E46">
         <v>2017</v>
       </c>
       <c r="F46" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G46" t="s">
-        <v>97</v>
+        <v>164</v>
       </c>
       <c r="H46" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="I46" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J46" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>2</v>
       </c>
@@ -2282,28 +2297,28 @@
         <v>45</v>
       </c>
       <c r="C47" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E47">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F47" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G47" t="s">
-        <v>98</v>
+        <v>163</v>
       </c>
       <c r="H47" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="I47" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J47" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>2</v>
       </c>
@@ -2311,28 +2326,28 @@
         <v>45</v>
       </c>
       <c r="C48" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="E48">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F48" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G48" t="s">
-        <v>99</v>
+        <v>164</v>
       </c>
       <c r="H48" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="I48" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J48" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>2</v>
       </c>
@@ -2340,28 +2355,28 @@
         <v>45</v>
       </c>
       <c r="C49" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E49">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="F49" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G49" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
       <c r="H49" t="s">
-        <v>84</v>
+        <v>162</v>
       </c>
       <c r="I49" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J49" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>2</v>
       </c>
@@ -2369,28 +2384,28 @@
         <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="E50">
         <v>2017</v>
       </c>
       <c r="F50" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G50" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H50" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="I50" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J50" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>2</v>
       </c>
@@ -2398,28 +2413,28 @@
         <v>45</v>
       </c>
       <c r="C51" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="E51">
         <v>2017</v>
       </c>
       <c r="F51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="G51" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H51" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="I51" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J51" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>2</v>
       </c>
@@ -2427,28 +2442,28 @@
         <v>45</v>
       </c>
       <c r="C52" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E52">
         <v>2017</v>
       </c>
       <c r="F52" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="G52" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H52" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="I52" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J52" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>2</v>
       </c>
@@ -2456,28 +2471,28 @@
         <v>45</v>
       </c>
       <c r="C53" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E53">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F53" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="G53" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="H53" t="s">
         <v>84</v>
       </c>
       <c r="I53" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J53" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>2</v>
       </c>
@@ -2485,28 +2500,28 @@
         <v>45</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="E54">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G54" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="H54" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="I54" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J54" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>2</v>
       </c>
@@ -2514,28 +2529,28 @@
         <v>45</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E55">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="G55" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="H55" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="I55" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J55" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>2</v>
       </c>
@@ -2543,28 +2558,28 @@
         <v>45</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E56">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F56" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="G56" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
       <c r="H56" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="I56" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J56" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>2</v>
       </c>
@@ -2572,28 +2587,28 @@
         <v>45</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E57">
         <v>2012</v>
       </c>
       <c r="F57" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="G57" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="H57" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="I57" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J57" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>2</v>
       </c>
@@ -2601,28 +2616,28 @@
         <v>45</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E58">
         <v>2012</v>
       </c>
       <c r="F58" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="G58" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="H58" t="s">
-        <v>101</v>
+        <v>84</v>
       </c>
       <c r="I58" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J58" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>2</v>
       </c>
@@ -2630,28 +2645,28 @@
         <v>45</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="E59">
         <v>2012</v>
       </c>
       <c r="F59" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="G59" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="H59" t="s">
-        <v>103</v>
+        <v>84</v>
       </c>
       <c r="I59" t="s">
-        <v>136</v>
+        <v>196</v>
       </c>
       <c r="J59" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>2</v>
       </c>
@@ -2659,129 +2674,144 @@
         <v>45</v>
       </c>
       <c r="C60" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E60">
         <v>2012</v>
       </c>
       <c r="F60" t="s">
+        <v>100</v>
+      </c>
+      <c r="G60" t="s">
+        <v>100</v>
+      </c>
+      <c r="H60" t="s">
+        <v>84</v>
+      </c>
+      <c r="I60" t="s">
+        <v>196</v>
+      </c>
+      <c r="J60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>2</v>
+      </c>
+      <c r="B61">
+        <v>45</v>
+      </c>
+      <c r="C61" t="s">
+        <v>49</v>
+      </c>
+      <c r="E61">
+        <v>2012</v>
+      </c>
+      <c r="F61" t="s">
+        <v>105</v>
+      </c>
+      <c r="G61" t="s">
+        <v>105</v>
+      </c>
+      <c r="H61" t="s">
+        <v>101</v>
+      </c>
+      <c r="I61" t="s">
+        <v>196</v>
+      </c>
+      <c r="J61" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>2</v>
+      </c>
+      <c r="B62">
+        <v>45</v>
+      </c>
+      <c r="C62" t="s">
+        <v>50</v>
+      </c>
+      <c r="E62">
+        <v>2012</v>
+      </c>
+      <c r="F62" t="s">
+        <v>106</v>
+      </c>
+      <c r="G62" t="s">
+        <v>106</v>
+      </c>
+      <c r="H62" t="s">
+        <v>101</v>
+      </c>
+      <c r="I62" t="s">
+        <v>196</v>
+      </c>
+      <c r="J62" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>2</v>
+      </c>
+      <c r="B63">
+        <v>45</v>
+      </c>
+      <c r="C63" t="s">
+        <v>51</v>
+      </c>
+      <c r="E63">
+        <v>2012</v>
+      </c>
+      <c r="F63" t="s">
+        <v>107</v>
+      </c>
+      <c r="G63" t="s">
+        <v>107</v>
+      </c>
+      <c r="H63" t="s">
+        <v>103</v>
+      </c>
+      <c r="I63" t="s">
+        <v>196</v>
+      </c>
+      <c r="J63" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64">
+        <v>2</v>
+      </c>
+      <c r="B64">
+        <v>45</v>
+      </c>
+      <c r="C64" t="s">
+        <v>52</v>
+      </c>
+      <c r="E64">
+        <v>2012</v>
+      </c>
+      <c r="F64" t="s">
         <v>108</v>
       </c>
-      <c r="G60" t="s">
+      <c r="G64" t="s">
         <v>108</v>
       </c>
-      <c r="H60" t="s">
+      <c r="H64" t="s">
         <v>103</v>
       </c>
-      <c r="I60" t="s">
-        <v>136</v>
-      </c>
-      <c r="J60" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>2</v>
-      </c>
-      <c r="B61">
-        <v>8</v>
-      </c>
-      <c r="C61" t="s">
-        <v>182</v>
-      </c>
-      <c r="F61" t="s">
-        <v>184</v>
-      </c>
-      <c r="G61" t="s">
-        <v>176</v>
-      </c>
-      <c r="I61" t="s">
-        <v>136</v>
-      </c>
-      <c r="J61" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>2</v>
-      </c>
-      <c r="B62">
-        <v>8</v>
-      </c>
-      <c r="C62" t="s">
-        <v>53</v>
-      </c>
-      <c r="F62" t="s">
-        <v>177</v>
-      </c>
-      <c r="G62" t="s">
-        <v>176</v>
-      </c>
-      <c r="H62" t="s">
-        <v>84</v>
-      </c>
-      <c r="I62" t="s">
-        <v>137</v>
-      </c>
-      <c r="J62" t="s">
-        <v>138</v>
-      </c>
-      <c r="K62" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>2</v>
-      </c>
-      <c r="B63">
-        <v>8</v>
-      </c>
-      <c r="C63" t="s">
-        <v>181</v>
-      </c>
-      <c r="F63" t="s">
-        <v>185</v>
-      </c>
-      <c r="G63" t="s">
-        <v>174</v>
-      </c>
-      <c r="I63" t="s">
-        <v>136</v>
-      </c>
-      <c r="J63" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>2</v>
-      </c>
-      <c r="B64">
-        <v>8</v>
-      </c>
-      <c r="C64" t="s">
-        <v>180</v>
-      </c>
-      <c r="F64" t="s">
-        <v>178</v>
-      </c>
-      <c r="G64" t="s">
-        <v>174</v>
-      </c>
       <c r="I64" t="s">
-        <v>137</v>
+        <v>196</v>
       </c>
       <c r="J64" t="s">
         <v>138</v>
       </c>
-      <c r="K64" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>2</v>
       </c>
@@ -2789,13 +2819,13 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F65" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G65" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="I65" t="s">
         <v>136</v>
@@ -2804,7 +2834,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>2</v>
       </c>
@@ -2812,13 +2842,13 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F66" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G66" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="H66" t="s">
         <v>84</v>
@@ -2830,30 +2860,24 @@
         <v>138</v>
       </c>
       <c r="K66" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>2</v>
       </c>
       <c r="B67">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>55</v>
-      </c>
-      <c r="D67" t="s">
-        <v>56</v>
+        <v>181</v>
       </c>
       <c r="F67" t="s">
-        <v>109</v>
+        <v>185</v>
       </c>
       <c r="G67" t="s">
-        <v>109</v>
-      </c>
-      <c r="H67" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="I67" t="s">
         <v>136</v>
@@ -2862,56 +2886,47 @@
         <v>138</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>2</v>
       </c>
       <c r="B68">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>55</v>
-      </c>
-      <c r="D68" t="s">
-        <v>57</v>
+        <v>180</v>
       </c>
       <c r="F68" t="s">
-        <v>110</v>
+        <v>178</v>
       </c>
       <c r="G68" t="s">
-        <v>110</v>
-      </c>
-      <c r="H68" t="s">
-        <v>134</v>
+        <v>174</v>
       </c>
       <c r="I68" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J68" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K68" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>2</v>
       </c>
       <c r="B69">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>193</v>
-      </c>
-      <c r="D69" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="F69" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="G69" t="s">
-        <v>195</v>
-      </c>
-      <c r="H69" t="s">
-        <v>134</v>
+        <v>175</v>
       </c>
       <c r="I69" t="s">
         <v>136</v>
@@ -2920,120 +2935,114 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>2</v>
       </c>
       <c r="B70">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>58</v>
-      </c>
-      <c r="E70">
-        <v>2017</v>
+        <v>54</v>
       </c>
       <c r="F70" t="s">
-        <v>121</v>
+        <v>179</v>
       </c>
       <c r="G70" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
       <c r="H70" t="s">
         <v>84</v>
       </c>
       <c r="I70" t="s">
+        <v>137</v>
+      </c>
+      <c r="J70" t="s">
+        <v>138</v>
+      </c>
+      <c r="K70" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>2</v>
+      </c>
+      <c r="B71">
+        <v>42</v>
+      </c>
+      <c r="C71" t="s">
+        <v>55</v>
+      </c>
+      <c r="D71" t="s">
+        <v>56</v>
+      </c>
+      <c r="F71" t="s">
+        <v>109</v>
+      </c>
+      <c r="G71" t="s">
+        <v>109</v>
+      </c>
+      <c r="H71" t="s">
+        <v>134</v>
+      </c>
+      <c r="I71" t="s">
         <v>136</v>
       </c>
-      <c r="J70" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71">
-        <v>2</v>
-      </c>
-      <c r="B71">
-        <v>41</v>
-      </c>
-      <c r="C71" t="s">
-        <v>59</v>
-      </c>
-      <c r="E71">
-        <v>2017</v>
-      </c>
-      <c r="F71" t="s">
-        <v>111</v>
-      </c>
-      <c r="G71" t="s">
-        <v>166</v>
-      </c>
-      <c r="H71" t="s">
-        <v>84</v>
-      </c>
-      <c r="I71" t="s">
-        <v>137</v>
-      </c>
       <c r="J71" t="s">
         <v>138</v>
       </c>
-      <c r="K71" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>2</v>
       </c>
       <c r="B72">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C72" t="s">
-        <v>60</v>
-      </c>
-      <c r="E72">
-        <v>2017</v>
+        <v>55</v>
+      </c>
+      <c r="D72" t="s">
+        <v>57</v>
       </c>
       <c r="F72" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="G72" t="s">
-        <v>166</v>
+        <v>110</v>
       </c>
       <c r="H72" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="I72" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J72" t="s">
-        <v>139</v>
-      </c>
-      <c r="K72" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>2</v>
       </c>
       <c r="B73">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
-      </c>
-      <c r="E73">
-        <v>2017</v>
+        <v>193</v>
+      </c>
+      <c r="D73" t="s">
+        <v>194</v>
       </c>
       <c r="F73" t="s">
-        <v>123</v>
+        <v>195</v>
       </c>
       <c r="G73" t="s">
-        <v>167</v>
+        <v>195</v>
       </c>
       <c r="H73" t="s">
-        <v>84</v>
+        <v>134</v>
       </c>
       <c r="I73" t="s">
         <v>136</v>
@@ -3042,7 +3051,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>2</v>
       </c>
@@ -3050,31 +3059,28 @@
         <v>41</v>
       </c>
       <c r="C74" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="E74">
         <v>2017</v>
       </c>
       <c r="F74" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G74" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H74" t="s">
         <v>84</v>
       </c>
       <c r="I74" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J74" t="s">
         <v>138</v>
       </c>
-      <c r="K74" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>2</v>
       </c>
@@ -3082,16 +3088,16 @@
         <v>41</v>
       </c>
       <c r="C75" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="E75">
         <v>2017</v>
       </c>
       <c r="F75" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G75" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H75" t="s">
         <v>84</v>
@@ -3100,13 +3106,13 @@
         <v>137</v>
       </c>
       <c r="J75" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K75" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>2</v>
       </c>
@@ -3114,28 +3120,31 @@
         <v>41</v>
       </c>
       <c r="C76" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E76">
         <v>2017</v>
       </c>
       <c r="F76" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G76" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H76" t="s">
         <v>84</v>
       </c>
       <c r="I76" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J76" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="K76" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>2</v>
       </c>
@@ -3143,31 +3152,28 @@
         <v>41</v>
       </c>
       <c r="C77" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E77">
         <v>2017</v>
       </c>
       <c r="F77" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G77" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H77" t="s">
         <v>84</v>
       </c>
       <c r="I77" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J77" t="s">
         <v>138</v>
       </c>
-      <c r="K77" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>2</v>
       </c>
@@ -3175,16 +3181,16 @@
         <v>41</v>
       </c>
       <c r="C78" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E78">
         <v>2017</v>
       </c>
       <c r="F78" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="G78" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H78" t="s">
         <v>84</v>
@@ -3193,91 +3199,91 @@
         <v>137</v>
       </c>
       <c r="J78" t="s">
+        <v>138</v>
+      </c>
+      <c r="K78" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A79">
+        <v>2</v>
+      </c>
+      <c r="B79">
+        <v>41</v>
+      </c>
+      <c r="C79" t="s">
+        <v>63</v>
+      </c>
+      <c r="E79">
+        <v>2017</v>
+      </c>
+      <c r="F79" t="s">
+        <v>124</v>
+      </c>
+      <c r="G79" t="s">
+        <v>167</v>
+      </c>
+      <c r="H79" t="s">
+        <v>84</v>
+      </c>
+      <c r="I79" t="s">
+        <v>137</v>
+      </c>
+      <c r="J79" t="s">
         <v>139</v>
       </c>
-      <c r="K78" t="s">
+      <c r="K79" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A80">
+        <v>2</v>
+      </c>
+      <c r="B80">
+        <v>41</v>
+      </c>
+      <c r="C80" t="s">
+        <v>64</v>
+      </c>
+      <c r="E80">
+        <v>2017</v>
+      </c>
+      <c r="F80" t="s">
         <v>125</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79">
-        <v>99</v>
-      </c>
-      <c r="B79">
-        <v>99</v>
-      </c>
-      <c r="C79" t="s">
-        <v>77</v>
-      </c>
-      <c r="E79">
-        <v>2012</v>
-      </c>
-      <c r="F79" t="s">
-        <v>121</v>
-      </c>
-      <c r="G79" t="s">
-        <v>166</v>
-      </c>
-      <c r="H79" t="s">
-        <v>84</v>
-      </c>
-      <c r="I79" t="s">
+      <c r="G80" t="s">
+        <v>168</v>
+      </c>
+      <c r="H80" t="s">
+        <v>84</v>
+      </c>
+      <c r="I80" t="s">
         <v>136</v>
       </c>
-      <c r="J79" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80">
-        <v>99</v>
-      </c>
-      <c r="B80">
-        <v>99</v>
-      </c>
-      <c r="C80" t="s">
-        <v>75</v>
-      </c>
-      <c r="E80">
-        <v>2012</v>
-      </c>
-      <c r="F80" t="s">
-        <v>111</v>
-      </c>
-      <c r="G80" t="s">
-        <v>166</v>
-      </c>
-      <c r="H80" t="s">
-        <v>84</v>
-      </c>
-      <c r="I80" t="s">
-        <v>137</v>
-      </c>
       <c r="J80" t="s">
         <v>138</v>
       </c>
-      <c r="K80" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>99</v>
+        <v>2</v>
       </c>
       <c r="B81">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="C81" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="E81">
-        <v>2012</v>
+        <v>2017</v>
       </c>
       <c r="F81" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="G81" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="H81" t="s">
         <v>84</v>
@@ -3286,42 +3292,45 @@
         <v>137</v>
       </c>
       <c r="J81" t="s">
+        <v>138</v>
+      </c>
+      <c r="K81" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A82">
+        <v>2</v>
+      </c>
+      <c r="B82">
+        <v>41</v>
+      </c>
+      <c r="C82" t="s">
+        <v>66</v>
+      </c>
+      <c r="E82">
+        <v>2017</v>
+      </c>
+      <c r="F82" t="s">
+        <v>126</v>
+      </c>
+      <c r="G82" t="s">
+        <v>168</v>
+      </c>
+      <c r="H82" t="s">
+        <v>84</v>
+      </c>
+      <c r="I82" t="s">
+        <v>137</v>
+      </c>
+      <c r="J82" t="s">
         <v>139</v>
       </c>
-      <c r="K81" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82">
-        <v>99</v>
-      </c>
-      <c r="B82">
-        <v>99</v>
-      </c>
-      <c r="C82" t="s">
-        <v>78</v>
-      </c>
-      <c r="E82">
-        <v>2012</v>
-      </c>
-      <c r="F82" t="s">
-        <v>123</v>
-      </c>
-      <c r="G82" t="s">
-        <v>167</v>
-      </c>
-      <c r="H82" t="s">
-        <v>84</v>
-      </c>
-      <c r="I82" t="s">
-        <v>136</v>
-      </c>
-      <c r="J82" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="K82" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>99</v>
       </c>
@@ -3329,31 +3338,28 @@
         <v>99</v>
       </c>
       <c r="C83" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E83">
         <v>2012</v>
       </c>
       <c r="F83" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
       <c r="G83" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H83" t="s">
         <v>84</v>
       </c>
       <c r="I83" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J83" t="s">
         <v>138</v>
       </c>
-      <c r="K83" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>99</v>
       </c>
@@ -3361,16 +3367,16 @@
         <v>99</v>
       </c>
       <c r="C84" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="E84">
         <v>2012</v>
       </c>
       <c r="F84" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="G84" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="H84" t="s">
         <v>84</v>
@@ -3379,13 +3385,13 @@
         <v>137</v>
       </c>
       <c r="J84" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="K84" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>99</v>
       </c>
@@ -3393,28 +3399,31 @@
         <v>99</v>
       </c>
       <c r="C85" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="E85">
         <v>2012</v>
       </c>
       <c r="F85" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="G85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="H85" t="s">
         <v>84</v>
       </c>
       <c r="I85" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="J85" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+      <c r="K85" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>99</v>
       </c>
@@ -3422,31 +3431,28 @@
         <v>99</v>
       </c>
       <c r="C86" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E86">
         <v>2012</v>
       </c>
       <c r="F86" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="G86" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H86" t="s">
         <v>84</v>
       </c>
       <c r="I86" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J86" t="s">
         <v>138</v>
       </c>
-      <c r="K86" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>99</v>
       </c>
@@ -3454,16 +3460,16 @@
         <v>99</v>
       </c>
       <c r="C87" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E87">
         <v>2012</v>
       </c>
       <c r="F87" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="G87" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="H87" t="s">
         <v>84</v>
@@ -3472,9 +3478,134 @@
         <v>137</v>
       </c>
       <c r="J87" t="s">
+        <v>138</v>
+      </c>
+      <c r="K87" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>99</v>
+      </c>
+      <c r="B88">
+        <v>99</v>
+      </c>
+      <c r="C88" t="s">
+        <v>80</v>
+      </c>
+      <c r="E88">
+        <v>2012</v>
+      </c>
+      <c r="F88" t="s">
+        <v>124</v>
+      </c>
+      <c r="G88" t="s">
+        <v>167</v>
+      </c>
+      <c r="H88" t="s">
+        <v>84</v>
+      </c>
+      <c r="I88" t="s">
+        <v>137</v>
+      </c>
+      <c r="J88" t="s">
         <v>139</v>
       </c>
-      <c r="K87" t="s">
+      <c r="K88" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A89">
+        <v>99</v>
+      </c>
+      <c r="B89">
+        <v>99</v>
+      </c>
+      <c r="C89" t="s">
+        <v>81</v>
+      </c>
+      <c r="E89">
+        <v>2012</v>
+      </c>
+      <c r="F89" t="s">
+        <v>125</v>
+      </c>
+      <c r="G89" t="s">
+        <v>168</v>
+      </c>
+      <c r="H89" t="s">
+        <v>84</v>
+      </c>
+      <c r="I89" t="s">
+        <v>136</v>
+      </c>
+      <c r="J89" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A90">
+        <v>99</v>
+      </c>
+      <c r="B90">
+        <v>99</v>
+      </c>
+      <c r="C90" t="s">
+        <v>82</v>
+      </c>
+      <c r="E90">
+        <v>2012</v>
+      </c>
+      <c r="F90" t="s">
+        <v>113</v>
+      </c>
+      <c r="G90" t="s">
+        <v>168</v>
+      </c>
+      <c r="H90" t="s">
+        <v>84</v>
+      </c>
+      <c r="I90" t="s">
+        <v>137</v>
+      </c>
+      <c r="J90" t="s">
+        <v>138</v>
+      </c>
+      <c r="K90" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>99</v>
+      </c>
+      <c r="B91">
+        <v>99</v>
+      </c>
+      <c r="C91" t="s">
+        <v>83</v>
+      </c>
+      <c r="E91">
+        <v>2012</v>
+      </c>
+      <c r="F91" t="s">
+        <v>126</v>
+      </c>
+      <c r="G91" t="s">
+        <v>168</v>
+      </c>
+      <c r="H91" t="s">
+        <v>84</v>
+      </c>
+      <c r="I91" t="s">
+        <v>137</v>
+      </c>
+      <c r="J91" t="s">
+        <v>139</v>
+      </c>
+      <c r="K91" t="s">
         <v>125</v>
       </c>
     </row>

</xml_diff>